<commit_message>
FINALIZADO DOCUMENTO INDIVIDUAL AUTOREFLEXION
</commit_message>
<xml_diff>
--- a/Fase 1/Evidencias Individuales/Araus_Bruno_1.3_APT122_AutoevaluaciónFase1.xlsx
+++ b/Fase 1/Evidencias Individuales/Araus_Bruno_1.3_APT122_AutoevaluaciónFase1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Melipilla\Documents\GitHub\Proyecto-PANAP\Fase 1\Evidencias Individuales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Desktop\PANAP\Proyecto-PANAP\Fase 1\Evidencias Individuales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82492A6-6CA8-4A7D-86A5-3D3E9D84CB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B589E4F2-A15E-4135-9CE6-90E90B958F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0163F3DC-111E-492F-9F90-07755503934C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{0163F3DC-111E-492F-9F90-07755503934C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="82">
   <si>
     <t>Indicador de Evaluación</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>No logrado (0%)</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -396,7 +399,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -507,11 +510,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -528,9 +614,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -540,12 +623,51 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -561,24 +683,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -588,47 +692,41 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -648,9 +746,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -688,7 +786,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -794,7 +892,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -936,7 +1034,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -946,8 +1044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D64B2826-5EC7-4E20-B24B-2D0AE56A4FD2}">
   <dimension ref="B2:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,37 +1064,37 @@
   <sheetData>
     <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="28" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="30"/>
-      <c r="C4" s="38" t="s">
+      <c r="B4" s="11"/>
+      <c r="C4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="19" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -1005,27 +1103,27 @@
       <c r="F4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="36"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
     </row>
     <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="31"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="2">
         <v>-0.3</v>
       </c>
       <c r="F5" s="2">
         <v>0</v>
       </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="16"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
     </row>
     <row r="6" spans="2:11" ht="90" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
@@ -1043,123 +1141,167 @@
       <c r="F6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="32">
         <v>5</v>
       </c>
+      <c r="H6" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
     </row>
     <row r="7" spans="2:11" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="20">
+      <c r="G7" s="33">
         <v>5</v>
       </c>
+      <c r="H7" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="7" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="21"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
     </row>
     <row r="9" spans="2:11" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
       <c r="F9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="22"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="33">
         <v>5</v>
       </c>
+      <c r="H10" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="21"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
     </row>
     <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
     </row>
     <row r="13" spans="2:11" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="20">
+      <c r="G13" s="33">
         <v>5</v>
       </c>
+      <c r="H13" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="7" t="s">
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="21"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
     </row>
     <row r="15" spans="2:11" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
       <c r="D15" s="5" t="s">
         <v>28</v>
       </c>
@@ -1169,7 +1311,11 @@
       <c r="F15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="22"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
     </row>
     <row r="16" spans="2:11" ht="90" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="4" t="s">
@@ -1187,11 +1333,17 @@
       <c r="F16" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="32">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" ht="90" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H16" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
+    </row>
+    <row r="17" spans="2:11" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>38</v>
       </c>
@@ -1207,39 +1359,55 @@
       <c r="F17" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="32">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="17" t="s">
+      <c r="H17" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+    </row>
+    <row r="18" spans="2:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="G18" s="20">
+      <c r="G18" s="33">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="22"/>
-    </row>
-    <row r="20" spans="2:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H18" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
+    </row>
+    <row r="19" spans="2:11" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+    </row>
+    <row r="20" spans="2:11" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
         <v>48</v>
       </c>
@@ -1255,51 +1423,71 @@
       <c r="F20" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="32">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B21" s="17" t="s">
+      <c r="H20" s="40"/>
+      <c r="I20" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+    </row>
+    <row r="21" spans="2:11" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B21" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="17" t="s">
+      <c r="E21" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="F21" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="G21" s="20">
+      <c r="G21" s="33">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="18"/>
-      <c r="C22" s="7" t="s">
+      <c r="H21" s="41"/>
+      <c r="I21" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="J21" s="41"/>
+      <c r="K21" s="41"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="22"/>
+      <c r="C22" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="21"/>
-    </row>
-    <row r="23" spans="2:7" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="19"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+    </row>
+    <row r="23" spans="2:11" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="23"/>
       <c r="C23" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="22"/>
-    </row>
-    <row r="24" spans="2:7" ht="90" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="43"/>
+    </row>
+    <row r="24" spans="2:11" ht="90" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="4" t="s">
         <v>59</v>
       </c>
@@ -1315,11 +1503,17 @@
       <c r="F24" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="32">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H24" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+    </row>
+    <row r="25" spans="2:11" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
         <v>64</v>
       </c>
@@ -1335,67 +1529,139 @@
       <c r="F25" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="32">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B26" s="17" t="s">
+      <c r="H25" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+    </row>
+    <row r="26" spans="2:11" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B26" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="23" t="s">
+      <c r="D26" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="E26" s="23" t="s">
+      <c r="E26" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G26" s="26">
+      <c r="G26" s="36">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="B27" s="18"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="8" t="s">
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="41"/>
+      <c r="K26" s="41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="B27" s="22"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="G27" s="27"/>
-    </row>
-    <row r="28" spans="2:7" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="19"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="9" t="s">
+      <c r="G27" s="37"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="42"/>
+    </row>
+    <row r="28" spans="2:11" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="23"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="G28" s="28"/>
-    </row>
-    <row r="29" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="12" t="s">
+      <c r="G28" s="38"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
+      <c r="K28" s="43"/>
+    </row>
+    <row r="29" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="10">
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="39">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="11"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="40"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="64">
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="I26:I28"/>
+    <mergeCell ref="J26:J28"/>
+    <mergeCell ref="K26:K28"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="K21:K23"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="J13:J15"/>
+    <mergeCell ref="K13:K15"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="K10:K12"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="K3:K5"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
     <mergeCell ref="G10:G12"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:F3"/>
@@ -1412,30 +1678,6 @@
     <mergeCell ref="D10:D12"/>
     <mergeCell ref="E10:E12"/>
     <mergeCell ref="F10:F12"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="K3:K5"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="G26:G28"/>
-    <mergeCell ref="B13:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>